<commit_message>
Update and minor fix
</commit_message>
<xml_diff>
--- a/BOM REV 0.5.xlsx
+++ b/BOM REV 0.5.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFB091A-04A7-469F-806E-3BC5D63A3A60}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B79D594-84FF-440F-96E4-0EFC7CEBC8DF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="248">
   <si>
     <t xml:space="preserve">    C3</t>
   </si>
@@ -760,17 +760,17 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Rechargable 5V power bank REV 0.5 - BOM</t>
-  </si>
-  <si>
     <t>&gt;  R4, R10, R11, R14</t>
+  </si>
+  <si>
+    <t>Rechargeable 5V power bank REV 0.5 - BOM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -778,13 +778,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -804,7 +817,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1157,8 +1170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,9 +1189,9 @@
     <col min="13" max="13" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2507,7 +2520,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B34" s="1">
         <v>4</v>

</xml_diff>